<commit_message>
Criação do one class classifier
</commit_message>
<xml_diff>
--- a/results/results.xlsx
+++ b/results/results.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25601"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ronal\PycharmProjects\ppca-md\results\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93395E53-0D29-49B4-8205-A3BEA43398A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet r:id="rId1" sheetId="1" name="Página1"/>
+    <sheet name="Página1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="38">
   <si>
     <t>Experimento</t>
   </si>
@@ -125,12 +131,15 @@
   </si>
   <si>
     <t>One-Class Selo com otimização</t>
+  </si>
+  <si>
+    <t>OneClassSVM - RBF Kernel</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0.00000"/>
   </numFmts>
@@ -191,59 +200,53 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+  <cellXfs count="14">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="4" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="4" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" builtinId="0" name="Normal"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -254,10 +257,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="000000"/>
@@ -295,71 +298,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Times New Roman" script="Arab"/>
-        <a:font typeface="Times New Roman" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="MoolBoran" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Times New Roman" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Arial" script="Arab"/>
-        <a:font typeface="Arial" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="DaunPenh" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Arial" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -387,7 +390,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
@@ -410,11 +413,11 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="9500"/>
@@ -423,13 +426,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -439,7 +442,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -448,7 +451,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -457,7 +460,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -465,10 +468,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot rev="0" lon="0" lat="0"/>
+              <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig dir="t" rig="threePt">
-              <a:rot rev="1200000" lon="0" lat="0"/>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -533,33 +536,29 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:N15"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" style="11" width="29.862142857142857" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="11" width="49.005" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="12" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="12" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="12" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="12" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="12" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="12" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="12" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="11" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="13" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="12" max="12" style="11" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="13" max="13" style="14" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="14" max="14" style="11" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="29.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="49" bestFit="1" customWidth="1"/>
+    <col min="3" max="9" width="13.5546875" style="11" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.5546875" style="12" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.5546875" style="13" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
+    <row r="1" spans="1:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -603,7 +602,7 @@
         <v>13</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
+    <row r="2" spans="1:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>14</v>
       </c>
@@ -611,25 +610,25 @@
         <v>15</v>
       </c>
       <c r="C2" s="6">
-        <v>0.8532</v>
+        <v>0.85319999999999996</v>
       </c>
       <c r="D2" s="6">
         <v>0</v>
       </c>
       <c r="E2" s="6">
-        <v>0.8532</v>
+        <v>0.85319999999999996</v>
       </c>
       <c r="F2" s="6">
-        <v>0.8646</v>
+        <v>0.86460000000000004</v>
       </c>
       <c r="G2" s="6">
-        <v>0.853</v>
+        <v>0.85299999999999998</v>
       </c>
       <c r="H2" s="6">
-        <v>0.7799</v>
+        <v>0.77990000000000004</v>
       </c>
       <c r="I2" s="6">
-        <v>0.7847</v>
+        <v>0.78469999999999995</v>
       </c>
       <c r="J2" s="5" t="s">
         <v>16</v>
@@ -647,7 +646,7 @@
         <v>18</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
+    <row r="3" spans="1:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>19</v>
       </c>
@@ -655,22 +654,22 @@
         <v>15</v>
       </c>
       <c r="C3" s="6">
-        <v>0.8344</v>
+        <v>0.83440000000000003</v>
       </c>
       <c r="D3" s="6">
         <v>0</v>
       </c>
       <c r="E3" s="6">
-        <v>0.8344</v>
+        <v>0.83440000000000003</v>
       </c>
       <c r="F3" s="6">
-        <v>0.8544</v>
+        <v>0.85440000000000005</v>
       </c>
       <c r="G3" s="6">
-        <v>0.8317</v>
+        <v>0.83169999999999999</v>
       </c>
       <c r="H3" s="6">
-        <v>0.7516</v>
+        <v>0.75160000000000005</v>
       </c>
       <c r="I3" s="6">
         <v>0.7611</v>
@@ -691,7 +690,7 @@
         <v>18</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
+    <row r="4" spans="1:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>20</v>
       </c>
@@ -699,25 +698,25 @@
         <v>15</v>
       </c>
       <c r="C4" s="6">
-        <v>0.8763</v>
+        <v>0.87629999999999997</v>
       </c>
       <c r="D4" s="6">
-        <v>0.8884</v>
+        <v>0.88839999999999997</v>
       </c>
       <c r="E4" s="6">
-        <v>0.9245</v>
+        <v>0.92449999999999999</v>
       </c>
       <c r="F4" s="6">
-        <v>0.7577</v>
+        <v>0.75770000000000004</v>
       </c>
       <c r="G4" s="6">
-        <v>0.8329</v>
+        <v>0.83289999999999997</v>
       </c>
       <c r="H4" s="6">
-        <v>0.7362</v>
+        <v>0.73619999999999997</v>
       </c>
       <c r="I4" s="6">
-        <v>0.7454</v>
+        <v>0.74539999999999995</v>
       </c>
       <c r="J4" s="5" t="s">
         <v>16</v>
@@ -735,7 +734,7 @@
         <v>18</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
+    <row r="5" spans="1:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>21</v>
       </c>
@@ -743,25 +742,25 @@
         <v>22</v>
       </c>
       <c r="C5" s="6">
-        <v>0.8994</v>
+        <v>0.89939999999999998</v>
       </c>
       <c r="D5" s="6">
-        <v>0.9679</v>
+        <v>0.96789999999999998</v>
       </c>
       <c r="E5" s="6">
-        <v>0.8868</v>
+        <v>0.88680000000000003</v>
       </c>
       <c r="F5" s="6">
         <v>0.8246</v>
       </c>
       <c r="G5" s="6">
-        <v>0.8545</v>
+        <v>0.85450000000000004</v>
       </c>
       <c r="H5" s="6">
-        <v>0.7778</v>
+        <v>0.77780000000000005</v>
       </c>
       <c r="I5" s="6">
-        <v>0.779</v>
+        <v>0.77900000000000003</v>
       </c>
       <c r="J5" s="5" t="s">
         <v>6</v>
@@ -779,7 +778,7 @@
         <v>18</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
+    <row r="6" spans="1:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>23</v>
       </c>
@@ -787,22 +786,22 @@
         <v>24</v>
       </c>
       <c r="C6" s="6">
-        <v>0.8637</v>
+        <v>0.86370000000000002</v>
       </c>
       <c r="D6" s="6">
-        <v>0.9275</v>
+        <v>0.92749999999999999</v>
       </c>
       <c r="E6" s="6">
-        <v>0.5912</v>
+        <v>0.59119999999999995</v>
       </c>
       <c r="F6" s="6">
         <v>1</v>
       </c>
       <c r="G6" s="6">
-        <v>0.7431</v>
+        <v>0.74309999999999998</v>
       </c>
       <c r="H6" s="6">
-        <v>0.6585</v>
+        <v>0.65849999999999997</v>
       </c>
       <c r="I6" s="6">
         <v>0.7006</v>
@@ -823,7 +822,7 @@
         <v>18</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
+    <row r="7" spans="1:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>25</v>
       </c>
@@ -831,25 +830,25 @@
         <v>26</v>
       </c>
       <c r="C7" s="6">
-        <v>0.8616</v>
+        <v>0.86160000000000003</v>
       </c>
       <c r="D7" s="6">
-        <v>0.961</v>
+        <v>0.96099999999999997</v>
       </c>
       <c r="E7" s="6">
-        <v>0.5912</v>
+        <v>0.59119999999999995</v>
       </c>
       <c r="F7" s="6">
-        <v>0.9895</v>
+        <v>0.98950000000000005</v>
       </c>
       <c r="G7" s="6">
-        <v>0.7402</v>
+        <v>0.74019999999999997</v>
       </c>
       <c r="H7" s="6">
-        <v>0.6538</v>
+        <v>0.65380000000000005</v>
       </c>
       <c r="I7" s="6">
-        <v>0.6941</v>
+        <v>0.69410000000000005</v>
       </c>
       <c r="J7" s="5" t="s">
         <v>6</v>
@@ -867,7 +866,7 @@
         <v>18</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
+    <row r="8" spans="1:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>27</v>
       </c>
@@ -875,25 +874,25 @@
         <v>28</v>
       </c>
       <c r="C8" s="6">
-        <v>0.9182</v>
+        <v>0.91820000000000002</v>
       </c>
       <c r="D8" s="6">
-        <v>0.9135</v>
+        <v>0.91349999999999998</v>
       </c>
       <c r="E8" s="6">
-        <v>0.8994</v>
+        <v>0.89939999999999998</v>
       </c>
       <c r="F8" s="6">
-        <v>0.8614</v>
+        <v>0.86140000000000005</v>
       </c>
       <c r="G8" s="6">
         <v>0.88</v>
       </c>
       <c r="H8" s="6">
-        <v>0.818</v>
+        <v>0.81799999999999995</v>
       </c>
       <c r="I8" s="6">
-        <v>0.8185</v>
+        <v>0.81850000000000001</v>
       </c>
       <c r="J8" s="5" t="s">
         <v>16</v>
@@ -911,7 +910,7 @@
         <v>18</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
+    <row r="9" spans="1:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
         <v>29</v>
       </c>
@@ -919,25 +918,25 @@
         <v>30</v>
       </c>
       <c r="C9" s="6">
-        <v>0.935</v>
+        <v>0.93500000000000005</v>
       </c>
       <c r="D9" s="6">
-        <v>0.9732</v>
+        <v>0.97319999999999995</v>
       </c>
       <c r="E9" s="6">
         <v>0.8679</v>
       </c>
       <c r="F9" s="6">
-        <v>0.9324</v>
+        <v>0.93240000000000001</v>
       </c>
       <c r="G9" s="6">
-        <v>0.899</v>
+        <v>0.89900000000000002</v>
       </c>
       <c r="H9" s="6">
-        <v>0.8512</v>
+        <v>0.85119999999999996</v>
       </c>
       <c r="I9" s="6">
-        <v>0.8524</v>
+        <v>0.85240000000000005</v>
       </c>
       <c r="J9" s="5" t="s">
         <v>6</v>
@@ -955,25 +954,37 @@
         <v>18</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
+    <row r="10" spans="1:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="B10" s="5"/>
-      <c r="C10" s="6"/>
+      <c r="B10" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C10" s="6">
+        <v>0.67710000000000004</v>
+      </c>
       <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="6"/>
+      <c r="E10" s="6">
+        <v>0.68</v>
+      </c>
+      <c r="F10" s="6">
+        <v>0.7</v>
+      </c>
+      <c r="G10" s="6">
+        <v>0.68</v>
+      </c>
       <c r="H10" s="6"/>
       <c r="I10" s="6"/>
-      <c r="J10" s="5"/>
+      <c r="J10" s="5" t="s">
+        <v>16</v>
+      </c>
       <c r="K10" s="9"/>
       <c r="L10" s="5"/>
       <c r="M10" s="10"/>
       <c r="N10" s="5"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
+    <row r="11" spans="1:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
         <v>32</v>
       </c>
@@ -991,25 +1002,37 @@
       <c r="M11" s="10"/>
       <c r="N11" s="5"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
+    <row r="12" spans="1:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="B12" s="5"/>
-      <c r="C12" s="6"/>
+      <c r="B12" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C12" s="6">
+        <v>0.61</v>
+      </c>
       <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="6"/>
-      <c r="G12" s="6"/>
+      <c r="E12" s="6">
+        <v>0.61</v>
+      </c>
+      <c r="F12" s="6">
+        <v>0.59</v>
+      </c>
+      <c r="G12" s="6">
+        <v>0.6</v>
+      </c>
       <c r="H12" s="6"/>
       <c r="I12" s="6"/>
-      <c r="J12" s="5"/>
+      <c r="J12" s="5" t="s">
+        <v>16</v>
+      </c>
       <c r="K12" s="9"/>
       <c r="L12" s="5"/>
       <c r="M12" s="10"/>
       <c r="N12" s="5"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
+    <row r="13" spans="1:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
         <v>34</v>
       </c>
@@ -1027,25 +1050,37 @@
       <c r="M13" s="10"/>
       <c r="N13" s="5"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
+    <row r="14" spans="1:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="B14" s="5"/>
-      <c r="C14" s="6"/>
+      <c r="B14" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C14" s="6">
+        <v>0.52829999999999999</v>
+      </c>
       <c r="D14" s="6"/>
-      <c r="E14" s="6"/>
-      <c r="F14" s="6"/>
-      <c r="G14" s="6"/>
+      <c r="E14" s="6">
+        <v>0.53</v>
+      </c>
+      <c r="F14" s="6">
+        <v>0.59</v>
+      </c>
+      <c r="G14" s="6">
+        <v>0.54</v>
+      </c>
       <c r="H14" s="6"/>
       <c r="I14" s="6"/>
-      <c r="J14" s="5"/>
+      <c r="J14" s="5" t="s">
+        <v>16</v>
+      </c>
       <c r="K14" s="9"/>
       <c r="L14" s="5"/>
       <c r="M14" s="10"/>
       <c r="N14" s="5"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="20.25">
+    <row r="15" spans="1:14" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
         <v>36</v>
       </c>

</xml_diff>

<commit_message>
Otimização do one class classifier
</commit_message>
<xml_diff>
--- a/results/results.xlsx
+++ b/results/results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ronal\PycharmProjects\ppca-md\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93395E53-0D29-49B4-8205-A3BEA43398A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84E6ACE9-5FCB-4303-BFD3-2C89CF8F03BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="40">
   <si>
     <t>Experimento</t>
   </si>
@@ -133,7 +133,13 @@
     <t>One-Class Selo com otimização</t>
   </si>
   <si>
-    <t>OneClassSVM - RBF Kernel</t>
+    <t>OneClassSVM - RBF Kernel - mu = 0,1</t>
+  </si>
+  <si>
+    <t>OneClassSVM - RBF Kernel - mu = 0,0002</t>
+  </si>
+  <si>
+    <t>mu = 0,0002</t>
   </si>
 </sst>
 </file>
@@ -543,7 +549,7 @@
   <dimension ref="A1:N15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="A13" sqref="A13:XFD13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -988,15 +994,27 @@
       <c r="A11" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="B11" s="5"/>
-      <c r="C11" s="6"/>
+      <c r="B11" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C11" s="6">
+        <v>0.6855</v>
+      </c>
       <c r="D11" s="6"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="6"/>
-      <c r="G11" s="6"/>
+      <c r="E11" s="6">
+        <v>0.69</v>
+      </c>
+      <c r="F11" s="6">
+        <v>0.74</v>
+      </c>
+      <c r="G11" s="6">
+        <v>0.57999999999999996</v>
+      </c>
       <c r="H11" s="6"/>
       <c r="I11" s="6"/>
-      <c r="J11" s="5"/>
+      <c r="J11" s="5" t="s">
+        <v>39</v>
+      </c>
       <c r="K11" s="9"/>
       <c r="L11" s="5"/>
       <c r="M11" s="10"/>
@@ -1036,15 +1054,27 @@
       <c r="A13" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="B13" s="5"/>
-      <c r="C13" s="6"/>
+      <c r="B13" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C13" s="6">
+        <v>0.67500000000000004</v>
+      </c>
       <c r="D13" s="6"/>
-      <c r="E13" s="6"/>
-      <c r="F13" s="6"/>
-      <c r="G13" s="6"/>
+      <c r="E13" s="6">
+        <v>0.68</v>
+      </c>
+      <c r="F13" s="6">
+        <v>0.7</v>
+      </c>
+      <c r="G13" s="6">
+        <v>0.56000000000000005</v>
+      </c>
       <c r="H13" s="6"/>
       <c r="I13" s="6"/>
-      <c r="J13" s="5"/>
+      <c r="J13" s="5" t="s">
+        <v>39</v>
+      </c>
       <c r="K13" s="9"/>
       <c r="L13" s="5"/>
       <c r="M13" s="10"/>
@@ -1084,15 +1114,27 @@
       <c r="A15" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="B15" s="5"/>
-      <c r="C15" s="6"/>
+      <c r="B15" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C15" s="6">
+        <v>0.6603</v>
+      </c>
       <c r="D15" s="6"/>
-      <c r="E15" s="6"/>
-      <c r="F15" s="6"/>
-      <c r="G15" s="6"/>
+      <c r="E15" s="6">
+        <v>0.66</v>
+      </c>
+      <c r="F15" s="6">
+        <v>0.62</v>
+      </c>
+      <c r="G15" s="6">
+        <v>0.61</v>
+      </c>
       <c r="H15" s="6"/>
       <c r="I15" s="6"/>
-      <c r="J15" s="5"/>
+      <c r="J15" s="5" t="s">
+        <v>39</v>
+      </c>
       <c r="K15" s="9"/>
       <c r="L15" s="5"/>
       <c r="M15" s="10"/>

</xml_diff>